<commit_message>
falta crear el excel
</commit_message>
<xml_diff>
--- a/horario_generado.xlsx
+++ b/horario_generado.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,7 +464,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>08:15-09:45</t>
+          <t>08:31-09:50</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr"/>
@@ -477,20 +477,32 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10:00-11:30</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr"/>
-      <c r="C3" s="1" t="inlineStr"/>
+          <t>10:01-10:40</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>DSY1105-004D</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>DSY1104-003D</t>
+        </is>
+      </c>
       <c r="D3" s="1" t="inlineStr"/>
-      <c r="E3" s="1" t="inlineStr"/>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>DSY1104-003D</t>
+        </is>
+      </c>
       <c r="F3" s="1" t="inlineStr"/>
       <c r="G3" s="1" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>11:45-13:15</t>
+          <t>10:41-11:20</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr"/>
@@ -503,7 +515,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>14:30-16:00</t>
+          <t>11:31-12:10</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr"/>
@@ -516,7 +528,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:15-17:45</t>
+          <t>13:41-14:20</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr"/>
@@ -529,7 +541,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:00-19:30</t>
+          <t>14:31-15:10</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr"/>
@@ -542,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>19:45-21:15</t>
+          <t>16:15-17:45</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr"/>
@@ -552,6 +564,58 @@
       <c r="F8" s="1" t="inlineStr"/>
       <c r="G8" s="1" t="inlineStr"/>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>18:00-19:30</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr"/>
+      <c r="C9" s="1" t="inlineStr"/>
+      <c r="D9" s="1" t="inlineStr"/>
+      <c r="E9" s="1" t="inlineStr"/>
+      <c r="F9" s="1" t="inlineStr"/>
+      <c r="G9" s="1" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>19:01-20:20</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr"/>
+      <c r="C10" s="1" t="inlineStr"/>
+      <c r="D10" s="1" t="inlineStr"/>
+      <c r="E10" s="1" t="inlineStr"/>
+      <c r="F10" s="1" t="inlineStr"/>
+      <c r="G10" s="1" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>20:31-21:10</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr"/>
+      <c r="C11" s="1" t="inlineStr"/>
+      <c r="D11" s="1" t="inlineStr"/>
+      <c r="E11" s="1" t="inlineStr"/>
+      <c r="F11" s="1" t="inlineStr"/>
+      <c r="G11" s="1" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>21:11-22:30</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr"/>
+      <c r="C12" s="1" t="inlineStr"/>
+      <c r="D12" s="1" t="inlineStr"/>
+      <c r="E12" s="1" t="inlineStr"/>
+      <c r="F12" s="1" t="inlineStr"/>
+      <c r="G12" s="1" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>